<commit_message>
Modificaciones luego de la semana 3
</commit_message>
<xml_diff>
--- a/Horario.xlsx
+++ b/Horario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Informática\Horario - Informática\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EEE704-3854-4B27-A374-C38CBC20DE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACD2D40-EBEA-4203-9504-29349CEBDBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>Estudiar para el parcial de cálculo</t>
   </si>
   <si>
-    <t>Se hicieron modificaciones en la segunda semana para ajustar los tiempos a los parciales que se programaron (26/02/2023).</t>
-  </si>
-  <si>
     <t>Taller de cálculo de la universidad</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Último repaso para los parciales de Cálculo y Física</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se hicieron modificaciones en la segunda semana para ajustar los tiempos a los parciales que se programaron (26/02/2023). La semana transcurrió con relativa normalidad y los horarios propuestos fueron tal como se planearon. (07/03/2023) </t>
   </si>
 </sst>
 </file>
@@ -385,8 +385,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,23 +415,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN35" sqref="AN35"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,53 +737,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="P2" s="21" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="P2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AD2" s="16" t="s">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AD2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="16"/>
-      <c r="AQ2" s="16"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -814,21 +814,21 @@
       <c r="N3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="6" t="s">
         <v>0</v>
@@ -901,19 +901,19 @@
       <c r="N4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
       <c r="AD4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1000,19 +1000,19 @@
       <c r="N5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
       <c r="AD5" s="3" t="s">
         <v>39</v>
       </c>
@@ -1043,10 +1043,10 @@
       <c r="AM5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="19" t="s">
+      <c r="AN5" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AO5" s="17" t="s">
+      <c r="AO5" s="22" t="s">
         <v>31</v>
       </c>
       <c r="AP5" s="3" t="s">
@@ -1099,19 +1099,19 @@
       <c r="N6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
       <c r="AD6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1142,8 +1142,8 @@
       <c r="AM6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AN6" s="20"/>
-      <c r="AO6" s="18"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="23"/>
       <c r="AP6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1186,19 +1186,19 @@
       <c r="L7" s="12"/>
       <c r="M7" s="14"/>
       <c r="N7" s="12"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="25"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
       <c r="AD7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1265,19 +1265,19 @@
       <c r="L8" s="12"/>
       <c r="M8" s="14"/>
       <c r="N8" s="12"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="12"/>
       <c r="AF8" s="3" t="s">
@@ -1306,53 +1306,53 @@
       <c r="D9" s="2"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="P12" s="21" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="P12" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AD12" s="23" t="s">
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="16"/>
+      <c r="AD12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="24"/>
-      <c r="AG12" s="24"/>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="24"/>
-      <c r="AK12" s="24"/>
-      <c r="AL12" s="24"/>
-      <c r="AM12" s="24"/>
-      <c r="AN12" s="24"/>
-      <c r="AO12" s="24"/>
-      <c r="AP12" s="24"/>
-      <c r="AQ12" s="24"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
     </row>
     <row r="13" spans="1:43" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
@@ -1383,21 +1383,21 @@
       <c r="N13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="6" t="s">
         <v>0</v>
@@ -1470,19 +1470,19 @@
       <c r="N14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="25"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
       <c r="AD14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1569,19 +1569,19 @@
       <c r="N15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
       <c r="AD15" s="3" t="s">
         <v>4</v>
       </c>
@@ -1668,19 +1668,19 @@
       <c r="N16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
-      <c r="AA16" s="25"/>
-      <c r="AB16" s="25"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
       <c r="AD16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1759,19 +1759,19 @@
       <c r="L17" s="12"/>
       <c r="M17" s="14"/>
       <c r="N17" s="12"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="21"/>
       <c r="AD17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1830,19 +1830,19 @@
       <c r="L18" s="12"/>
       <c r="M18" s="14"/>
       <c r="N18" s="12"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
       <c r="AD18" s="5"/>
       <c r="AE18" s="12"/>
       <c r="AF18" s="3" t="s">
@@ -1871,53 +1871,53 @@
       <c r="AQ18" s="12"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="P22" s="21" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="P22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AD22" s="23" t="s">
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="16"/>
+      <c r="AD22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
-      <c r="AG22" s="24"/>
-      <c r="AH22" s="24"/>
-      <c r="AI22" s="24"/>
-      <c r="AJ22" s="24"/>
-      <c r="AK22" s="24"/>
-      <c r="AL22" s="24"/>
-      <c r="AM22" s="24"/>
-      <c r="AN22" s="24"/>
-      <c r="AO22" s="24"/>
-      <c r="AP22" s="24"/>
-      <c r="AQ22" s="24"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="20"/>
+      <c r="AG22" s="20"/>
+      <c r="AH22" s="20"/>
+      <c r="AI22" s="20"/>
+      <c r="AJ22" s="20"/>
+      <c r="AK22" s="20"/>
+      <c r="AL22" s="20"/>
+      <c r="AM22" s="20"/>
+      <c r="AN22" s="20"/>
+      <c r="AO22" s="20"/>
+      <c r="AP22" s="20"/>
+      <c r="AQ22" s="20"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
@@ -1949,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
@@ -2341,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="AE27" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF27" s="4" t="s">
         <v>3</v>
@@ -2409,11 +2409,11 @@
       <c r="AA28" s="26"/>
       <c r="AB28" s="26"/>
       <c r="AD28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE28" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="AE28" s="15" t="s">
-        <v>57</v>
-      </c>
       <c r="AF28" s="3" t="s">
         <v>7</v>
       </c>
@@ -2421,10 +2421,10 @@
         <v>1</v>
       </c>
       <c r="AH28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AI28" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ28" s="3" t="s">
         <v>22</v>
@@ -2443,18 +2443,18 @@
       <c r="AD29" s="3"/>
       <c r="AE29" s="15"/>
       <c r="AF29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AG29" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH29" s="5"/>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK29" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="AK29" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="AL29" s="5"/>
       <c r="AM29" s="13"/>
@@ -2464,37 +2464,37 @@
       <c r="AQ29" s="12"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A33" s="23">
+      <c r="A33" s="19">
         <v>0</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="P33" s="21" t="s">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="P33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="21"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="21"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
@@ -2525,19 +2525,19 @@
       <c r="N34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22"/>
-      <c r="W34" s="22"/>
-      <c r="X34" s="22"/>
-      <c r="Y34" s="22"/>
-      <c r="Z34" s="22"/>
-      <c r="AA34" s="22"/>
-      <c r="AB34" s="22"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -2582,19 +2582,19 @@
       <c r="N35" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="22"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22"/>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
-      <c r="Z35" s="22"/>
-      <c r="AA35" s="22"/>
-      <c r="AB35" s="22"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
     </row>
     <row r="36" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
@@ -2639,19 +2639,19 @@
       <c r="N36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
-      <c r="U36" s="22"/>
-      <c r="V36" s="22"/>
-      <c r="W36" s="22"/>
-      <c r="X36" s="22"/>
-      <c r="Y36" s="22"/>
-      <c r="Z36" s="22"/>
-      <c r="AA36" s="22"/>
-      <c r="AB36" s="22"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
     </row>
     <row r="37" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -2696,19 +2696,19 @@
       <c r="N37" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
-      <c r="V37" s="22"/>
-      <c r="W37" s="22"/>
-      <c r="X37" s="22"/>
-      <c r="Y37" s="22"/>
-      <c r="Z37" s="22"/>
-      <c r="AA37" s="22"/>
-      <c r="AB37" s="22"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="17"/>
+      <c r="AB37" s="17"/>
     </row>
     <row r="38" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -2745,19 +2745,19 @@
       <c r="L38" s="12"/>
       <c r="M38" s="14"/>
       <c r="N38" s="12"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="22"/>
-      <c r="AA38" s="22"/>
-      <c r="AB38" s="22"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+      <c r="Y38" s="17"/>
+      <c r="Z38" s="17"/>
+      <c r="AA38" s="17"/>
+      <c r="AB38" s="17"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
@@ -2782,22 +2782,29 @@
       <c r="L39" s="12"/>
       <c r="M39" s="14"/>
       <c r="N39" s="12"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="S39" s="22"/>
-      <c r="T39" s="22"/>
-      <c r="U39" s="22"/>
-      <c r="V39" s="22"/>
-      <c r="W39" s="22"/>
-      <c r="X39" s="22"/>
-      <c r="Y39" s="22"/>
-      <c r="Z39" s="22"/>
-      <c r="AA39" s="22"/>
-      <c r="AB39" s="22"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+      <c r="AA39" s="17"/>
+      <c r="AB39" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AD2:AQ2"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="AN5:AN6"/>
+    <mergeCell ref="P22:AB22"/>
+    <mergeCell ref="P23:AB28"/>
+    <mergeCell ref="AD12:AQ12"/>
+    <mergeCell ref="AD22:AQ22"/>
     <mergeCell ref="P33:AB33"/>
     <mergeCell ref="P34:AB39"/>
     <mergeCell ref="A2:N2"/>
@@ -2808,13 +2815,6 @@
     <mergeCell ref="P3:AB8"/>
     <mergeCell ref="P12:AB12"/>
     <mergeCell ref="P13:AB18"/>
-    <mergeCell ref="AD2:AQ2"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="AN5:AN6"/>
-    <mergeCell ref="P22:AB22"/>
-    <mergeCell ref="P23:AB28"/>
-    <mergeCell ref="AD12:AQ12"/>
-    <mergeCell ref="AD22:AQ22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>